<commit_message>
added biomass data for 2019-2020 and updated the produciton data, feed, escapees, and mortality data; deleted redundant tables
</commit_message>
<xml_diff>
--- a/prep/administrative/fylker_kommuner_2019_2020_changes.xlsx
+++ b/prep/administrative/fylker_kommuner_2019_2020_changes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11010"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marinaespinasse/github/coastrisk/prep/administrative/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{397841D4-ABA7-0D47-8D5D-0A744DA24DE3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EB4A5EF-9D2B-F643-B026-2D7594497F7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3540" yWindow="4180" windowWidth="29900" windowHeight="19020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2040" yWindow="6360" windowWidth="33600" windowHeight="18720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Kommuner og fylker 2019-2020" sheetId="1" r:id="rId1"/>
@@ -1779,9 +1779,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:H426"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A324" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1821,7 +1824,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -1847,7 +1850,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -1873,7 +1876,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>1</v>
       </c>
@@ -1899,7 +1902,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>1</v>
       </c>
@@ -1925,7 +1928,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <v>1</v>
       </c>
@@ -1951,7 +1954,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
         <v>1</v>
       </c>
@@ -1977,7 +1980,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
         <v>1</v>
       </c>
@@ -2003,7 +2006,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
         <v>1</v>
       </c>
@@ -2029,7 +2032,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
         <v>1</v>
       </c>
@@ -2055,7 +2058,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
         <v>1</v>
       </c>
@@ -2081,7 +2084,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" s="3">
         <v>1</v>
       </c>
@@ -2107,7 +2110,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" s="3">
         <v>1</v>
       </c>
@@ -2133,7 +2136,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" s="3">
         <v>1</v>
       </c>
@@ -2159,7 +2162,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" s="3">
         <v>1</v>
       </c>
@@ -2185,7 +2188,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" s="3">
         <v>1</v>
       </c>
@@ -2211,7 +2214,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" s="3">
         <v>1</v>
       </c>
@@ -2237,7 +2240,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" s="3">
         <v>1</v>
       </c>
@@ -2263,7 +2266,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" s="3">
         <v>1</v>
       </c>
@@ -2289,7 +2292,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20" s="3">
         <v>2</v>
       </c>
@@ -2315,7 +2318,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" s="3">
         <v>2</v>
       </c>
@@ -2341,7 +2344,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22" s="3">
         <v>2</v>
       </c>
@@ -2367,7 +2370,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" s="3">
         <v>2</v>
       </c>
@@ -2393,7 +2396,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" s="3">
         <v>2</v>
       </c>
@@ -2419,7 +2422,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25" s="3">
         <v>2</v>
       </c>
@@ -2445,7 +2448,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" s="3">
         <v>2</v>
       </c>
@@ -2471,7 +2474,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" s="3">
         <v>2</v>
       </c>
@@ -2497,7 +2500,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28" s="3">
         <v>2</v>
       </c>
@@ -2523,7 +2526,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" s="3">
         <v>2</v>
       </c>
@@ -2549,7 +2552,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30" s="3">
         <v>2</v>
       </c>
@@ -2575,7 +2578,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31" s="3">
         <v>2</v>
       </c>
@@ -2601,7 +2604,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32" s="3">
         <v>2</v>
       </c>
@@ -2627,7 +2630,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33" s="3">
         <v>2</v>
       </c>
@@ -2653,7 +2656,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34" s="3">
         <v>2</v>
       </c>
@@ -2679,7 +2682,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35" s="3">
         <v>2</v>
       </c>
@@ -2705,7 +2708,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36" s="3">
         <v>2</v>
       </c>
@@ -2731,7 +2734,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37" s="3">
         <v>2</v>
       </c>
@@ -2757,7 +2760,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A38" s="3">
         <v>2</v>
       </c>
@@ -2783,7 +2786,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39" s="3">
         <v>2</v>
       </c>
@@ -2809,7 +2812,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A40" s="3">
         <v>2</v>
       </c>
@@ -2835,7 +2838,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A41" s="3">
         <v>2</v>
       </c>
@@ -2861,7 +2864,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A42" s="3">
         <v>3</v>
       </c>
@@ -2887,7 +2890,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43" s="3">
         <v>4</v>
       </c>
@@ -2913,7 +2916,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A44" s="3">
         <v>4</v>
       </c>
@@ -2939,7 +2942,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A45" s="3">
         <v>4</v>
       </c>
@@ -2965,7 +2968,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A46" s="3">
         <v>4</v>
       </c>
@@ -2991,7 +2994,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A47" s="3">
         <v>4</v>
       </c>
@@ -3017,7 +3020,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A48" s="3">
         <v>4</v>
       </c>
@@ -3043,7 +3046,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A49" s="3">
         <v>4</v>
       </c>
@@ -3069,7 +3072,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A50" s="3">
         <v>4</v>
       </c>
@@ -3095,7 +3098,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A51" s="3">
         <v>4</v>
       </c>
@@ -3121,7 +3124,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A52" s="3">
         <v>4</v>
       </c>
@@ -3147,7 +3150,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A53" s="3">
         <v>4</v>
       </c>
@@ -3173,7 +3176,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A54" s="3">
         <v>4</v>
       </c>
@@ -3199,7 +3202,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A55" s="3">
         <v>4</v>
       </c>
@@ -3225,7 +3228,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A56" s="3">
         <v>4</v>
       </c>
@@ -3251,7 +3254,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A57" s="3">
         <v>4</v>
       </c>
@@ -3277,7 +3280,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A58" s="3">
         <v>4</v>
       </c>
@@ -3303,7 +3306,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A59" s="3">
         <v>4</v>
       </c>
@@ -3329,7 +3332,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A60" s="3">
         <v>4</v>
       </c>
@@ -3355,7 +3358,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A61" s="3">
         <v>4</v>
       </c>
@@ -3381,7 +3384,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A62" s="3">
         <v>4</v>
       </c>
@@ -3407,7 +3410,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A63" s="3">
         <v>4</v>
       </c>
@@ -3433,7 +3436,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A64" s="3">
         <v>4</v>
       </c>
@@ -3459,7 +3462,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A65" s="3">
         <v>5</v>
       </c>
@@ -3485,7 +3488,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A66" s="3">
         <v>5</v>
       </c>
@@ -3511,7 +3514,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A67" s="3">
         <v>5</v>
       </c>
@@ -3537,7 +3540,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A68" s="3">
         <v>5</v>
       </c>
@@ -3563,7 +3566,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A69" s="3">
         <v>5</v>
       </c>
@@ -3589,7 +3592,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A70" s="3">
         <v>5</v>
       </c>
@@ -3615,7 +3618,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A71" s="3">
         <v>5</v>
       </c>
@@ -3641,7 +3644,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A72" s="3">
         <v>5</v>
       </c>
@@ -3667,7 +3670,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A73" s="3">
         <v>5</v>
       </c>
@@ -3693,7 +3696,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A74" s="3">
         <v>5</v>
       </c>
@@ -3719,7 +3722,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A75" s="3">
         <v>5</v>
       </c>
@@ -3745,7 +3748,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A76" s="3">
         <v>5</v>
       </c>
@@ -3771,7 +3774,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A77" s="3">
         <v>5</v>
       </c>
@@ -3797,7 +3800,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A78" s="3">
         <v>5</v>
       </c>
@@ -3823,7 +3826,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A79" s="3">
         <v>5</v>
       </c>
@@ -3849,7 +3852,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A80" s="3">
         <v>5</v>
       </c>
@@ -3875,7 +3878,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A81" s="3">
         <v>5</v>
       </c>
@@ -3901,7 +3904,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A82" s="3">
         <v>5</v>
       </c>
@@ -3927,7 +3930,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A83" s="3">
         <v>5</v>
       </c>
@@ -3953,7 +3956,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A84" s="3">
         <v>5</v>
       </c>
@@ -3979,7 +3982,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A85" s="3">
         <v>5</v>
       </c>
@@ -4005,7 +4008,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A86" s="3">
         <v>5</v>
       </c>
@@ -4031,7 +4034,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A87" s="3">
         <v>5</v>
       </c>
@@ -4057,7 +4060,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A88" s="3">
         <v>5</v>
       </c>
@@ -4083,7 +4086,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A89" s="3">
         <v>5</v>
       </c>
@@ -4109,7 +4112,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A90" s="3">
         <v>5</v>
       </c>
@@ -4135,7 +4138,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A91" s="3">
         <v>6</v>
       </c>
@@ -4161,7 +4164,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A92" s="3">
         <v>6</v>
       </c>
@@ -4187,7 +4190,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A93" s="3">
         <v>6</v>
       </c>
@@ -4213,7 +4216,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A94" s="3">
         <v>6</v>
       </c>
@@ -4239,7 +4242,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A95" s="3">
         <v>6</v>
       </c>
@@ -4265,7 +4268,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A96" s="3">
         <v>6</v>
       </c>
@@ -4291,7 +4294,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A97" s="3">
         <v>6</v>
       </c>
@@ -4317,7 +4320,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A98" s="3">
         <v>6</v>
       </c>
@@ -4343,7 +4346,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A99" s="3">
         <v>6</v>
       </c>
@@ -4369,7 +4372,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A100" s="3">
         <v>6</v>
       </c>
@@ -4395,7 +4398,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A101" s="3">
         <v>6</v>
       </c>
@@ -4421,7 +4424,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A102" s="3">
         <v>6</v>
       </c>
@@ -4447,7 +4450,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A103" s="3">
         <v>6</v>
       </c>
@@ -4473,7 +4476,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A104" s="3">
         <v>6</v>
       </c>
@@ -4499,7 +4502,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A105" s="3">
         <v>6</v>
       </c>
@@ -4525,7 +4528,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A106" s="3">
         <v>6</v>
       </c>
@@ -4551,7 +4554,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A107" s="3">
         <v>6</v>
       </c>
@@ -4577,7 +4580,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A108" s="3">
         <v>6</v>
       </c>
@@ -4603,7 +4606,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A109" s="3">
         <v>6</v>
       </c>
@@ -4629,7 +4632,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A110" s="3">
         <v>6</v>
       </c>
@@ -4655,7 +4658,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A111" s="3">
         <v>6</v>
       </c>
@@ -4681,7 +4684,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A112" s="3">
         <v>7</v>
       </c>
@@ -4707,7 +4710,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A113" s="3">
         <v>7</v>
       </c>
@@ -4733,7 +4736,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A114" s="3">
         <v>7</v>
       </c>
@@ -4759,7 +4762,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A115" s="3">
         <v>7</v>
       </c>
@@ -4785,7 +4788,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A116" s="3">
         <v>7</v>
       </c>
@@ -4811,7 +4814,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A117" s="3">
         <v>7</v>
       </c>
@@ -4837,7 +4840,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A118" s="3">
         <v>7</v>
       </c>
@@ -4863,7 +4866,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A119" s="3">
         <v>7</v>
       </c>
@@ -4889,7 +4892,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A120" s="3">
         <v>7</v>
       </c>
@@ -4915,7 +4918,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A121" s="3">
         <v>8</v>
       </c>
@@ -4941,7 +4944,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A122" s="3">
         <v>8</v>
       </c>
@@ -4967,7 +4970,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A123" s="3">
         <v>8</v>
       </c>
@@ -4993,7 +4996,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A124" s="3">
         <v>8</v>
       </c>
@@ -5019,7 +5022,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A125" s="3">
         <v>8</v>
       </c>
@@ -5045,7 +5048,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A126" s="3">
         <v>8</v>
       </c>
@@ -5071,7 +5074,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A127" s="3">
         <v>8</v>
       </c>
@@ -5097,7 +5100,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A128" s="3">
         <v>8</v>
       </c>
@@ -5123,7 +5126,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A129" s="3">
         <v>8</v>
       </c>
@@ -5149,7 +5152,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A130" s="3">
         <v>8</v>
       </c>
@@ -5175,7 +5178,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A131" s="3">
         <v>8</v>
       </c>
@@ -5201,7 +5204,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A132" s="3">
         <v>8</v>
       </c>
@@ -5227,7 +5230,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A133" s="3">
         <v>8</v>
       </c>
@@ -5253,7 +5256,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A134" s="3">
         <v>8</v>
       </c>
@@ -5279,7 +5282,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A135" s="3">
         <v>8</v>
       </c>
@@ -5305,7 +5308,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A136" s="3">
         <v>8</v>
       </c>
@@ -5331,7 +5334,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A137" s="3">
         <v>8</v>
       </c>
@@ -5357,7 +5360,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A138" s="3">
         <v>8</v>
       </c>
@@ -5383,7 +5386,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A139" s="3">
         <v>9</v>
       </c>
@@ -5409,7 +5412,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A140" s="3">
         <v>9</v>
       </c>
@@ -5435,7 +5438,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A141" s="3">
         <v>9</v>
       </c>
@@ -5461,7 +5464,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A142" s="3">
         <v>9</v>
       </c>
@@ -5487,7 +5490,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A143" s="3">
         <v>9</v>
       </c>
@@ -5513,7 +5516,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="144" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A144" s="3">
         <v>9</v>
       </c>
@@ -5539,7 +5542,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A145" s="3">
         <v>9</v>
       </c>
@@ -5565,7 +5568,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A146" s="3">
         <v>9</v>
       </c>
@@ -5591,7 +5594,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="147" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A147" s="3">
         <v>9</v>
       </c>
@@ -5617,7 +5620,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A148" s="3">
         <v>9</v>
       </c>
@@ -5643,7 +5646,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="149" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A149" s="3">
         <v>9</v>
       </c>
@@ -5669,7 +5672,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="150" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A150" s="3">
         <v>9</v>
       </c>
@@ -5695,7 +5698,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="151" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A151" s="3">
         <v>9</v>
       </c>
@@ -5721,7 +5724,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="152" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A152" s="3">
         <v>9</v>
       </c>
@@ -5747,7 +5750,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="153" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A153" s="3">
         <v>9</v>
       </c>
@@ -5773,7 +5776,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="154" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A154" s="3">
         <v>10</v>
       </c>
@@ -5799,7 +5802,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="155" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A155" s="3">
         <v>10</v>
       </c>
@@ -5851,7 +5854,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="157" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A157" s="3">
         <v>10</v>
       </c>
@@ -5877,7 +5880,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="158" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A158" s="3">
         <v>10</v>
       </c>
@@ -5903,7 +5906,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="159" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A159" s="3">
         <v>10</v>
       </c>
@@ -5929,7 +5932,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="160" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A160" s="3">
         <v>10</v>
       </c>
@@ -5955,7 +5958,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="161" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A161" s="3">
         <v>10</v>
       </c>
@@ -5981,7 +5984,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="162" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A162" s="3">
         <v>10</v>
       </c>
@@ -6007,7 +6010,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="163" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A163" s="3">
         <v>10</v>
       </c>
@@ -6033,7 +6036,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="164" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A164" s="3">
         <v>10</v>
       </c>
@@ -6059,7 +6062,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="165" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A165" s="3">
         <v>10</v>
       </c>
@@ -6085,7 +6088,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="166" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A166" s="3">
         <v>10</v>
       </c>
@@ -6111,7 +6114,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="167" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A167" s="3">
         <v>10</v>
       </c>
@@ -6137,7 +6140,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="168" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A168" s="3">
         <v>10</v>
       </c>
@@ -6163,7 +6166,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="169" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A169">
         <v>11</v>
       </c>
@@ -6189,7 +6192,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="170" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A170" s="3">
         <v>11</v>
       </c>
@@ -6215,7 +6218,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="171" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A171" s="3">
         <v>11</v>
       </c>
@@ -6241,7 +6244,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="172" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A172">
         <v>11</v>
       </c>
@@ -6267,7 +6270,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="173" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A173">
         <v>11</v>
       </c>
@@ -6293,7 +6296,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="174" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A174">
         <v>11</v>
       </c>
@@ -6319,7 +6322,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="175" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A175">
         <v>11</v>
       </c>
@@ -6345,7 +6348,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="176" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A176">
         <v>11</v>
       </c>
@@ -6371,7 +6374,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="177" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A177">
         <v>11</v>
       </c>
@@ -6397,7 +6400,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="178" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A178">
         <v>11</v>
       </c>
@@ -6423,7 +6426,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="179" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A179">
         <v>11</v>
       </c>
@@ -6449,7 +6452,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="180" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A180">
         <v>11</v>
       </c>
@@ -6475,7 +6478,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="181" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A181">
         <v>11</v>
       </c>
@@ -6501,7 +6504,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="182" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A182" s="3">
         <v>11</v>
       </c>
@@ -6527,7 +6530,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="183" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A183">
         <v>11</v>
       </c>
@@ -6553,7 +6556,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="184" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A184">
         <v>11</v>
       </c>
@@ -6579,7 +6582,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="185" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A185">
         <v>11</v>
       </c>
@@ -6605,7 +6608,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="186" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A186">
         <v>11</v>
       </c>
@@ -6631,7 +6634,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="187" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A187" s="3">
         <v>11</v>
       </c>
@@ -6657,7 +6660,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="188" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A188" s="3">
         <v>11</v>
       </c>
@@ -6683,7 +6686,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="189" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A189">
         <v>11</v>
       </c>
@@ -6709,7 +6712,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="190" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A190">
         <v>11</v>
       </c>
@@ -6735,7 +6738,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="191" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A191">
         <v>11</v>
       </c>
@@ -6761,7 +6764,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="192" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A192">
         <v>11</v>
       </c>
@@ -6787,7 +6790,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="193" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A193">
         <v>11</v>
       </c>
@@ -6813,7 +6816,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="194" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A194">
         <v>11</v>
       </c>
@@ -6839,7 +6842,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="195" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A195" s="3">
         <v>12</v>
       </c>
@@ -6865,7 +6868,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="196" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A196" s="3">
         <v>12</v>
       </c>
@@ -6891,7 +6894,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="197" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A197" s="3">
         <v>12</v>
       </c>
@@ -6917,7 +6920,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="198" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A198" s="3">
         <v>12</v>
       </c>
@@ -6943,7 +6946,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="199" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A199" s="3">
         <v>12</v>
       </c>
@@ -6969,7 +6972,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="200" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A200" s="3">
         <v>12</v>
       </c>
@@ -6995,7 +6998,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="201" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A201" s="3">
         <v>12</v>
       </c>
@@ -7021,7 +7024,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="202" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A202" s="3">
         <v>12</v>
       </c>
@@ -7047,7 +7050,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="203" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A203" s="3">
         <v>12</v>
       </c>
@@ -7073,7 +7076,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="204" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A204" s="3">
         <v>12</v>
       </c>
@@ -7099,7 +7102,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="205" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A205" s="3">
         <v>12</v>
       </c>
@@ -7125,7 +7128,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="206" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A206" s="3">
         <v>12</v>
       </c>
@@ -7151,7 +7154,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="207" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A207" s="3">
         <v>12</v>
       </c>
@@ -7177,7 +7180,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="208" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A208" s="3">
         <v>12</v>
       </c>
@@ -7203,7 +7206,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="209" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A209" s="3">
         <v>12</v>
       </c>
@@ -7229,7 +7232,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="210" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A210" s="3">
         <v>12</v>
       </c>
@@ -7255,7 +7258,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="211" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A211" s="3">
         <v>12</v>
       </c>
@@ -7281,7 +7284,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="212" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A212" s="3">
         <v>12</v>
       </c>
@@ -7307,7 +7310,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="213" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A213" s="3">
         <v>12</v>
       </c>
@@ -7333,7 +7336,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="214" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A214" s="3">
         <v>12</v>
       </c>
@@ -7359,7 +7362,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="215" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A215" s="3">
         <v>12</v>
       </c>
@@ -7385,7 +7388,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="216" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A216" s="3">
         <v>12</v>
       </c>
@@ -7411,7 +7414,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="217" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A217" s="3">
         <v>12</v>
       </c>
@@ -7437,7 +7440,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="218" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A218" s="3">
         <v>12</v>
       </c>
@@ -7463,7 +7466,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="219" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A219" s="3">
         <v>12</v>
       </c>
@@ -7489,7 +7492,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="220" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A220" s="3">
         <v>12</v>
       </c>
@@ -7515,7 +7518,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="221" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A221" s="3">
         <v>12</v>
       </c>
@@ -7541,7 +7544,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="222" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A222" s="3">
         <v>12</v>
       </c>
@@ -7567,7 +7570,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="223" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A223" s="3">
         <v>12</v>
       </c>
@@ -7593,7 +7596,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="224" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A224" s="3">
         <v>12</v>
       </c>
@@ -7619,7 +7622,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="225" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A225" s="3">
         <v>12</v>
       </c>
@@ -7645,7 +7648,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="226" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A226" s="3">
         <v>12</v>
       </c>
@@ -7671,7 +7674,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="227" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A227" s="3">
         <v>12</v>
       </c>
@@ -7697,7 +7700,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="228" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A228" s="3">
         <v>14</v>
       </c>
@@ -7723,7 +7726,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="229" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A229" s="3">
         <v>14</v>
       </c>
@@ -7749,7 +7752,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="230" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A230" s="3">
         <v>14</v>
       </c>
@@ -7775,7 +7778,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="231" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A231" s="3">
         <v>14</v>
       </c>
@@ -7801,7 +7804,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="232" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A232" s="3">
         <v>14</v>
       </c>
@@ -7827,7 +7830,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="233" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A233" s="3">
         <v>14</v>
       </c>
@@ -7853,7 +7856,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="234" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A234" s="3">
         <v>14</v>
       </c>
@@ -7879,7 +7882,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="235" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A235" s="3">
         <v>14</v>
       </c>
@@ -7905,7 +7908,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="236" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A236" s="3">
         <v>14</v>
       </c>
@@ -7931,7 +7934,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="237" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A237" s="3">
         <v>14</v>
       </c>
@@ -7957,7 +7960,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="238" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A238" s="3">
         <v>14</v>
       </c>
@@ -7983,7 +7986,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="239" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A239" s="3">
         <v>14</v>
       </c>
@@ -8009,7 +8012,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="240" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A240" s="3">
         <v>14</v>
       </c>
@@ -8035,7 +8038,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="241" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A241" s="3">
         <v>14</v>
       </c>
@@ -8061,7 +8064,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="242" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A242" s="3">
         <v>14</v>
       </c>
@@ -8087,7 +8090,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="243" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A243" s="3">
         <v>14</v>
       </c>
@@ -8113,7 +8116,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="244" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A244" s="3">
         <v>14</v>
       </c>
@@ -8139,7 +8142,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="245" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A245" s="3">
         <v>14</v>
       </c>
@@ -8165,7 +8168,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="246" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A246" s="3">
         <v>14</v>
       </c>
@@ -8191,7 +8194,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="247" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A247" s="3">
         <v>14</v>
       </c>
@@ -8217,7 +8220,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="248" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A248" s="3">
         <v>14</v>
       </c>
@@ -8243,7 +8246,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="249" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A249" s="3">
         <v>14</v>
       </c>
@@ -8269,7 +8272,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="250" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A250" s="3">
         <v>14</v>
       </c>
@@ -8295,7 +8298,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="251" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A251" s="3">
         <v>14</v>
       </c>
@@ -8321,7 +8324,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="252" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A252" s="3">
         <v>14</v>
       </c>
@@ -8347,7 +8350,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="253" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A253" s="3">
         <v>14</v>
       </c>
@@ -8373,7 +8376,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="254" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A254" s="3">
         <v>15</v>
       </c>
@@ -8399,7 +8402,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="255" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A255" s="3">
         <v>15</v>
       </c>
@@ -8425,7 +8428,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="256" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A256">
         <v>15</v>
       </c>
@@ -8451,7 +8454,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="257" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A257">
         <v>15</v>
       </c>
@@ -8477,7 +8480,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="258" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A258">
         <v>15</v>
       </c>
@@ -8503,7 +8506,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="259" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A259">
         <v>15</v>
       </c>
@@ -8529,7 +8532,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="260" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A260">
         <v>15</v>
       </c>
@@ -8555,7 +8558,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="261" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A261">
         <v>15</v>
       </c>
@@ -8581,7 +8584,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="262" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A262" s="3">
         <v>15</v>
       </c>
@@ -8607,7 +8610,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="263" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A263">
         <v>15</v>
       </c>
@@ -8633,7 +8636,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="264" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A264" s="3">
         <v>15</v>
       </c>
@@ -8659,7 +8662,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="265" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A265" s="3">
         <v>15</v>
       </c>
@@ -8685,7 +8688,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="266" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A266">
         <v>15</v>
       </c>
@@ -8711,7 +8714,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="267" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A267" s="3">
         <v>15</v>
       </c>
@@ -8737,7 +8740,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="268" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A268">
         <v>15</v>
       </c>
@@ -8763,7 +8766,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="269" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A269" s="3">
         <v>15</v>
       </c>
@@ -8789,7 +8792,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="270" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A270">
         <v>15</v>
       </c>
@@ -8815,7 +8818,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="271" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A271">
         <v>15</v>
       </c>
@@ -8841,7 +8844,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="272" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A272" s="3">
         <v>15</v>
       </c>
@@ -8867,7 +8870,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="273" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="273" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A273">
         <v>15</v>
       </c>
@@ -8893,7 +8896,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="274" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="274" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A274">
         <v>15</v>
       </c>
@@ -8919,7 +8922,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="275" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="275" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A275" s="3">
         <v>15</v>
       </c>
@@ -8945,7 +8948,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="276" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A276" s="3">
         <v>15</v>
       </c>
@@ -8971,7 +8974,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="277" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A277" s="3">
         <v>15</v>
       </c>
@@ -8997,7 +9000,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="278" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A278">
         <v>15</v>
       </c>
@@ -9023,7 +9026,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="279" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="279" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A279" s="3">
         <v>15</v>
       </c>
@@ -9049,7 +9052,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="280" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="280" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A280" s="3">
         <v>15</v>
       </c>
@@ -9075,7 +9078,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="281" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="281" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A281">
         <v>15</v>
       </c>
@@ -9101,7 +9104,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="282" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="282" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A282">
         <v>15</v>
       </c>
@@ -9127,7 +9130,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="283" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="283" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A283">
         <v>15</v>
       </c>
@@ -9153,7 +9156,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="284" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="284" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A284">
         <v>15</v>
       </c>
@@ -9179,7 +9182,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="285" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="285" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A285">
         <v>15</v>
       </c>
@@ -9205,7 +9208,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="286" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="286" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A286" s="3">
         <v>15</v>
       </c>
@@ -9231,7 +9234,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="287" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="287" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A287">
         <v>15</v>
       </c>
@@ -9257,7 +9260,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="288" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="288" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A288">
         <v>15</v>
       </c>
@@ -9283,7 +9286,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="289" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="289" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A289">
         <v>18</v>
       </c>
@@ -9309,7 +9312,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="290" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="290" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A290" s="3">
         <v>18</v>
       </c>
@@ -9335,7 +9338,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="291" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="291" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A291">
         <v>18</v>
       </c>
@@ -9361,7 +9364,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="292" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="292" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A292">
         <v>18</v>
       </c>
@@ -9387,7 +9390,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="293" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="293" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A293">
         <v>18</v>
       </c>
@@ -9413,7 +9416,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="294" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="294" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A294">
         <v>18</v>
       </c>
@@ -9439,7 +9442,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="295" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="295" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A295">
         <v>18</v>
       </c>
@@ -9465,7 +9468,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="296" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="296" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A296">
         <v>18</v>
       </c>
@@ -9491,7 +9494,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="297" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="297" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A297">
         <v>18</v>
       </c>
@@ -9517,7 +9520,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="298" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="298" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A298">
         <v>18</v>
       </c>
@@ -9543,7 +9546,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="299" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="299" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A299">
         <v>18</v>
       </c>
@@ -9569,7 +9572,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="300" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="300" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A300">
         <v>18</v>
       </c>
@@ -9595,7 +9598,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="301" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="301" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A301">
         <v>18</v>
       </c>
@@ -9621,7 +9624,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="302" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="302" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A302">
         <v>18</v>
       </c>
@@ -9647,7 +9650,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="303" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="303" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A303">
         <v>18</v>
       </c>
@@ -9673,7 +9676,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="304" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="304" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A304">
         <v>18</v>
       </c>
@@ -9699,7 +9702,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="305" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="305" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A305">
         <v>18</v>
       </c>
@@ -9725,7 +9728,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="306" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="306" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A306">
         <v>18</v>
       </c>
@@ -9751,7 +9754,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="307" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="307" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A307">
         <v>18</v>
       </c>
@@ -9777,7 +9780,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="308" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="308" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A308">
         <v>18</v>
       </c>
@@ -9803,7 +9806,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="309" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="309" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A309">
         <v>18</v>
       </c>
@@ -9829,7 +9832,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="310" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="310" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A310">
         <v>18</v>
       </c>
@@ -9855,7 +9858,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="311" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="311" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A311">
         <v>18</v>
       </c>
@@ -9881,7 +9884,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="312" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="312" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A312">
         <v>18</v>
       </c>
@@ -9907,7 +9910,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="313" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="313" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A313">
         <v>18</v>
       </c>
@@ -9933,7 +9936,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="314" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="314" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A314">
         <v>18</v>
       </c>
@@ -9959,7 +9962,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="315" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="315" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A315">
         <v>18</v>
       </c>
@@ -9985,7 +9988,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="316" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="316" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A316" s="3">
         <v>18</v>
       </c>
@@ -10011,7 +10014,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="317" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="317" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A317" s="3">
         <v>18</v>
       </c>
@@ -10037,7 +10040,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="318" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="318" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A318" s="3">
         <v>18</v>
       </c>
@@ -10063,7 +10066,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="319" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="319" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A319">
         <v>18</v>
       </c>
@@ -10089,7 +10092,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="320" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="320" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A320" s="3">
         <v>18</v>
       </c>
@@ -10115,7 +10118,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="321" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="321" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A321">
         <v>18</v>
       </c>
@@ -10141,7 +10144,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="322" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="322" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A322" s="3">
         <v>18</v>
       </c>
@@ -10167,7 +10170,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="323" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="323" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A323">
         <v>18</v>
       </c>
@@ -10193,7 +10196,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="324" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="324" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A324">
         <v>18</v>
       </c>
@@ -10219,7 +10222,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="325" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="325" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A325">
         <v>18</v>
       </c>
@@ -10245,7 +10248,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="326" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="326" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A326">
         <v>18</v>
       </c>
@@ -10271,7 +10274,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="327" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="327" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A327">
         <v>18</v>
       </c>
@@ -10297,7 +10300,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="328" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="328" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A328">
         <v>18</v>
       </c>
@@ -10323,7 +10326,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="329" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="329" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A329">
         <v>18</v>
       </c>
@@ -10349,7 +10352,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="330" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="330" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A330">
         <v>18</v>
       </c>
@@ -10375,7 +10378,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="331" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="331" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A331">
         <v>18</v>
       </c>
@@ -10401,7 +10404,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="332" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="332" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A332">
         <v>18</v>
       </c>
@@ -10427,7 +10430,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="333" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="333" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A333">
         <v>18</v>
       </c>
@@ -10453,7 +10456,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="334" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="334" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A334" s="3">
         <v>19</v>
       </c>
@@ -10479,7 +10482,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="335" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="335" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A335" s="3">
         <v>19</v>
       </c>
@@ -10505,7 +10508,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="336" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="336" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A336" s="3">
         <v>19</v>
       </c>
@@ -10531,7 +10534,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="337" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="337" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A337" s="3">
         <v>19</v>
       </c>
@@ -10557,7 +10560,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="338" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="338" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A338" s="3">
         <v>19</v>
       </c>
@@ -10583,7 +10586,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="339" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="339" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A339" s="3">
         <v>19</v>
       </c>
@@ -10609,7 +10612,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="340" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="340" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A340" s="3">
         <v>19</v>
       </c>
@@ -10635,7 +10638,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="341" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="341" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A341" s="3">
         <v>19</v>
       </c>
@@ -10661,7 +10664,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="342" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="342" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A342" s="3">
         <v>19</v>
       </c>
@@ -10687,7 +10690,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="343" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="343" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A343" s="3">
         <v>19</v>
       </c>
@@ -10713,7 +10716,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="344" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="344" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A344" s="3">
         <v>19</v>
       </c>
@@ -10739,7 +10742,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="345" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="345" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A345" s="3">
         <v>19</v>
       </c>
@@ -10765,7 +10768,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="346" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="346" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A346" s="3">
         <v>19</v>
       </c>
@@ -10791,7 +10794,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="347" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="347" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A347" s="3">
         <v>19</v>
       </c>
@@ -10817,7 +10820,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="348" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="348" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A348" s="3">
         <v>19</v>
       </c>
@@ -10843,7 +10846,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="349" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="349" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A349" s="3">
         <v>19</v>
       </c>
@@ -10869,7 +10872,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="350" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="350" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A350" s="3">
         <v>19</v>
       </c>
@@ -10895,7 +10898,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="351" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="351" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A351" s="3">
         <v>19</v>
       </c>
@@ -10921,7 +10924,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="352" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="352" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A352" s="3">
         <v>19</v>
       </c>
@@ -10947,7 +10950,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="353" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="353" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A353" s="3">
         <v>19</v>
       </c>
@@ -10973,7 +10976,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="354" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="354" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A354" s="3">
         <v>19</v>
       </c>
@@ -10999,7 +11002,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="355" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="355" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A355" s="3">
         <v>19</v>
       </c>
@@ -11025,7 +11028,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="356" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="356" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A356" s="3">
         <v>19</v>
       </c>
@@ -11051,7 +11054,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="357" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="357" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A357" s="3">
         <v>19</v>
       </c>
@@ -11077,7 +11080,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="358" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="358" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A358" s="3">
         <v>20</v>
       </c>
@@ -11103,7 +11106,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="359" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="359" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A359" s="3">
         <v>20</v>
       </c>
@@ -11129,7 +11132,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="360" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="360" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A360" s="3">
         <v>20</v>
       </c>
@@ -11155,7 +11158,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="361" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="361" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A361" s="3">
         <v>20</v>
       </c>
@@ -11181,7 +11184,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="362" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="362" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A362" s="3">
         <v>20</v>
       </c>
@@ -11207,7 +11210,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="363" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="363" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A363" s="3">
         <v>20</v>
       </c>
@@ -11233,7 +11236,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="364" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="364" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A364" s="3">
         <v>20</v>
       </c>
@@ -11259,7 +11262,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="365" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="365" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A365" s="3">
         <v>20</v>
       </c>
@@ -11285,7 +11288,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="366" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="366" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A366" s="3">
         <v>20</v>
       </c>
@@ -11311,7 +11314,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="367" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="367" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A367" s="3">
         <v>20</v>
       </c>
@@ -11337,7 +11340,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="368" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="368" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A368" s="3">
         <v>20</v>
       </c>
@@ -11363,7 +11366,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="369" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="369" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A369" s="3">
         <v>20</v>
       </c>
@@ -11389,7 +11392,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="370" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="370" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A370" s="3">
         <v>20</v>
       </c>
@@ -11415,7 +11418,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="371" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="371" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A371" s="3">
         <v>20</v>
       </c>
@@ -11441,7 +11444,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="372" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="372" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A372" s="3">
         <v>20</v>
       </c>
@@ -11467,7 +11470,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="373" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="373" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A373" s="3">
         <v>20</v>
       </c>
@@ -11493,7 +11496,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="374" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="374" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A374" s="3">
         <v>20</v>
       </c>
@@ -11519,7 +11522,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="375" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="375" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A375" s="3">
         <v>20</v>
       </c>
@@ -11545,7 +11548,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="376" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="376" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A376" s="3">
         <v>20</v>
       </c>
@@ -11571,7 +11574,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="377" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="377" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A377" s="3">
         <v>50</v>
       </c>
@@ -11597,7 +11600,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="378" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="378" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A378" s="3">
         <v>50</v>
       </c>
@@ -11623,7 +11626,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="379" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="379" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A379" s="3">
         <v>50</v>
       </c>
@@ -11649,7 +11652,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="380" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="380" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A380" s="3">
         <v>50</v>
       </c>
@@ -11675,7 +11678,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="381" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="381" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A381" s="3">
         <v>50</v>
       </c>
@@ -11701,7 +11704,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="382" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="382" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A382" s="3">
         <v>50</v>
       </c>
@@ -11727,7 +11730,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="383" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="383" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A383" s="3">
         <v>50</v>
       </c>
@@ -11753,7 +11756,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="384" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="384" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A384" s="3">
         <v>50</v>
       </c>
@@ -11779,7 +11782,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="385" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="385" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A385">
         <v>50</v>
       </c>
@@ -11805,7 +11808,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="386" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="386" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A386" s="3">
         <v>50</v>
       </c>
@@ -11831,7 +11834,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="387" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="387" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A387" s="3">
         <v>50</v>
       </c>
@@ -11857,7 +11860,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="388" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="388" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A388" s="3">
         <v>50</v>
       </c>
@@ -11883,7 +11886,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="389" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="389" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A389" s="3">
         <v>50</v>
       </c>
@@ -11909,7 +11912,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="390" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="390" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A390" s="3">
         <v>50</v>
       </c>
@@ -11935,7 +11938,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="391" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="391" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A391">
         <v>50</v>
       </c>
@@ -11961,7 +11964,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="392" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="392" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A392">
         <v>50</v>
       </c>
@@ -11987,7 +11990,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="393" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="393" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A393">
         <v>50</v>
       </c>
@@ -12013,7 +12016,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="394" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="394" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A394" s="3">
         <v>50</v>
       </c>
@@ -12039,7 +12042,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="395" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="395" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A395" s="3">
         <v>50</v>
       </c>
@@ -12065,7 +12068,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="396" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="396" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A396">
         <v>50</v>
       </c>
@@ -12091,7 +12094,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="397" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="397" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A397">
         <v>50</v>
       </c>
@@ -12117,7 +12120,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="398" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="398" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A398">
         <v>50</v>
       </c>
@@ -12143,7 +12146,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="399" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="399" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A399">
         <v>50</v>
       </c>
@@ -12169,7 +12172,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="400" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="400" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A400">
         <v>50</v>
       </c>
@@ -12195,7 +12198,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="401" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="401" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A401" s="3">
         <v>50</v>
       </c>
@@ -12221,7 +12224,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="402" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="402" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A402">
         <v>50</v>
       </c>
@@ -12247,7 +12250,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="403" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="403" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A403">
         <v>50</v>
       </c>
@@ -12273,7 +12276,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="404" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="404" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A404">
         <v>50</v>
       </c>
@@ -12299,7 +12302,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="405" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="405" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A405">
         <v>50</v>
       </c>
@@ -12325,7 +12328,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="406" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="406" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A406">
         <v>50</v>
       </c>
@@ -12351,7 +12354,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="407" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="407" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A407">
         <v>50</v>
       </c>
@@ -12377,7 +12380,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="408" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="408" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A408">
         <v>50</v>
       </c>
@@ -12403,7 +12406,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="409" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="409" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A409">
         <v>50</v>
       </c>
@@ -12429,7 +12432,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="410" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="410" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A410" s="3">
         <v>50</v>
       </c>
@@ -12455,7 +12458,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="411" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="411" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A411" s="3">
         <v>50</v>
       </c>
@@ -12481,7 +12484,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="412" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="412" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A412">
         <v>50</v>
       </c>
@@ -12507,7 +12510,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="413" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="413" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A413">
         <v>50</v>
       </c>
@@ -12533,7 +12536,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="414" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="414" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A414">
         <v>50</v>
       </c>
@@ -12559,7 +12562,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="415" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="415" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A415">
         <v>50</v>
       </c>
@@ -12585,7 +12588,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="416" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="416" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A416">
         <v>50</v>
       </c>
@@ -12611,7 +12614,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="417" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="417" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A417">
         <v>50</v>
       </c>
@@ -12637,7 +12640,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="418" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="418" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A418">
         <v>50</v>
       </c>
@@ -12663,7 +12666,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="419" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="419" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A419" s="3">
         <v>50</v>
       </c>
@@ -12689,7 +12692,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="420" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="420" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A420">
         <v>50</v>
       </c>
@@ -12715,7 +12718,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="421" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="421" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A421" s="3">
         <v>50</v>
       </c>
@@ -12741,7 +12744,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="422" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="422" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A422" s="3">
         <v>50</v>
       </c>
@@ -12767,7 +12770,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="423" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="423" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A423">
         <v>50</v>
       </c>
@@ -12793,7 +12796,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="424" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="424" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A424">
         <v>50</v>
       </c>
@@ -12819,7 +12822,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="425" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="425" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A425">
         <v>50</v>
       </c>
@@ -12845,7 +12848,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="426" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="426" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A426">
         <v>50</v>
       </c>
@@ -12872,10 +12875,12 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H426" xr:uid="{00000000-0009-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H426">
-      <sortCondition ref="C1:C426"/>
-    </sortState>
+  <autoFilter ref="A1:H426" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="6">
+      <filters>
+        <filter val="4206"/>
+      </filters>
+    </filterColumn>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
updated the analysis for most indicators of aquaculture, added some administrative data
</commit_message>
<xml_diff>
--- a/prep/administrative/fylker_kommuner_2019_2020_changes.xlsx
+++ b/prep/administrative/fylker_kommuner_2019_2020_changes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marinaespinasse/github/coastrisk/prep/administrative/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EB4A5EF-9D2B-F643-B026-2D7594497F7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C51E4A83-3AD9-C244-BCC7-83871655D5A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2040" yWindow="6360" windowWidth="33600" windowHeight="18720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6260" yWindow="13340" windowWidth="33600" windowHeight="18720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Kommuner og fylker 2019-2020" sheetId="1" r:id="rId1"/>
@@ -18,10 +18,19 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Kommuner og fylker 2019-2020'!$A$1:$H$426</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -5828,7 +5837,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="156" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A156" s="3">
         <v>10</v>
       </c>
@@ -8298,7 +8307,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="251" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A251" s="3">
         <v>14</v>
       </c>
@@ -12876,9 +12885,9 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:H426" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <filterColumn colId="6">
+    <filterColumn colId="2">
       <filters>
-        <filter val="4206"/>
+        <filter val="1444"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>